<commit_message>
Alteração planilha de tarefas
Alteração planilha de tarefas
</commit_message>
<xml_diff>
--- a/TCC/2º Encontro/Tarefas.xlsx
+++ b/TCC/2º Encontro/Tarefas.xlsx
@@ -544,12 +544,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -586,7 +585,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:7" hidden="1">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -632,7 +631,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -655,7 +654,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="22.5" hidden="1">
+    <row r="5" spans="1:7" ht="22.5">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -678,7 +677,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="22.5" hidden="1">
+    <row r="6" spans="1:7" ht="22.5">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -701,7 +700,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="33.75" hidden="1">
+    <row r="7" spans="1:7" ht="33.75">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -724,7 +723,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1">
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -747,7 +746,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1">
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -767,7 +766,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1">
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -790,7 +789,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1">
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -813,7 +812,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1">
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -836,7 +835,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1">
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>0</v>
       </c>
@@ -859,7 +858,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1">
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -882,7 +881,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1">
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>0</v>
       </c>
@@ -905,7 +904,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1">
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -928,7 +927,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1">
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>0</v>
       </c>
@@ -951,7 +950,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1">
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -974,7 +973,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="22.5" hidden="1">
+    <row r="19" spans="1:7" ht="22.5">
       <c r="A19" s="1">
         <v>0</v>
       </c>
@@ -997,7 +996,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1">
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1020,7 +1019,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1">
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -1043,7 +1042,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1">
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>0</v>
       </c>
@@ -1066,7 +1065,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1">
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>0</v>
       </c>
@@ -1089,7 +1088,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1">
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>0</v>
       </c>
@@ -1112,7 +1111,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="22.5" hidden="1">
+    <row r="25" spans="1:7" ht="22.5">
       <c r="A25" s="1">
         <v>0</v>
       </c>
@@ -1135,7 +1134,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="22.5" hidden="1">
+    <row r="26" spans="1:7" ht="22.5">
       <c r="A26" s="1">
         <v>0</v>
       </c>
@@ -1181,7 +1180,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1">
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
         <v>0</v>
       </c>
@@ -1204,7 +1203,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1">
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
         <v>0</v>
       </c>
@@ -1227,7 +1226,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1">
+    <row r="30" spans="1:7">
       <c r="A30" s="1">
         <v>0</v>
       </c>
@@ -1250,7 +1249,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1">
+    <row r="31" spans="1:7">
       <c r="A31" s="1">
         <v>0</v>
       </c>
@@ -1273,7 +1272,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1">
+    <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>0</v>
       </c>
@@ -1296,7 +1295,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1">
+    <row r="33" spans="1:7">
       <c r="A33" s="1">
         <v>0</v>
       </c>
@@ -1342,7 +1341,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1">
+    <row r="35" spans="1:7">
       <c r="A35" s="1">
         <v>0</v>
       </c>
@@ -1362,7 +1361,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1">
+    <row r="36" spans="1:7">
       <c r="A36" s="1">
         <v>0</v>
       </c>
@@ -1383,13 +1382,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G36">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Alexandre"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <sortState ref="A2:F33">
     <sortCondition descending="1" ref="A2"/>
   </sortState>

</xml_diff>

<commit_message>
Início de ajustes - Lista de características
Início de ajustes - Lista de características
</commit_message>
<xml_diff>
--- a/TCC/2º Encontro/Tarefas.xlsx
+++ b/TCC/2º Encontro/Tarefas.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tati\Desktop\Arquivos TCC\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="Tarefas" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tarefas!$A$1:$G$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tarefas!$A$1:$G$37</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -195,8 +190,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,9 +274,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -319,9 +314,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -353,27 +348,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -405,27 +382,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -598,15 +557,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -617,7 +577,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="5" customFormat="1" ht="22.5">
       <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
@@ -640,7 +600,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" hidden="1">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -663,7 +623,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" hidden="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -686,7 +646,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" hidden="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -709,7 +669,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="22.5">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -732,7 +692,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="22.5">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -755,7 +715,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="33.75">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -778,7 +738,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" hidden="1">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -801,7 +761,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" hidden="1">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -821,7 +781,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" hidden="1">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -844,7 +804,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" hidden="1">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -867,7 +827,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -890,7 +850,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" hidden="1">
       <c r="A13" s="1">
         <v>0</v>
       </c>
@@ -913,7 +873,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" hidden="1">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -936,7 +896,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" hidden="1">
       <c r="A15" s="1">
         <v>0</v>
       </c>
@@ -959,7 +919,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" hidden="1">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -982,7 +942,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>0</v>
       </c>
@@ -1005,7 +965,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -1028,7 +988,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="22.5">
       <c r="A19" s="1">
         <v>0</v>
       </c>
@@ -1051,7 +1011,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" hidden="1">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1074,7 +1034,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -1097,7 +1057,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>0</v>
       </c>
@@ -1120,7 +1080,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" hidden="1">
       <c r="A23" s="1">
         <v>0</v>
       </c>
@@ -1143,7 +1103,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" hidden="1">
       <c r="A24" s="1">
         <v>0</v>
       </c>
@@ -1166,7 +1126,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="22.5">
       <c r="A25" s="1">
         <v>0</v>
       </c>
@@ -1189,7 +1149,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="22.5" hidden="1">
       <c r="A26" s="1">
         <v>0</v>
       </c>
@@ -1212,7 +1172,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" hidden="1">
       <c r="A27" s="1">
         <v>0</v>
       </c>
@@ -1235,7 +1195,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" hidden="1">
       <c r="A28" s="1">
         <v>0</v>
       </c>
@@ -1258,7 +1218,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" hidden="1">
       <c r="A29" s="1">
         <v>0</v>
       </c>
@@ -1281,7 +1241,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" hidden="1">
       <c r="A30" s="1">
         <v>0</v>
       </c>
@@ -1304,7 +1264,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" s="1">
         <v>0</v>
       </c>
@@ -1327,7 +1287,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" hidden="1">
       <c r="A32" s="1">
         <v>0</v>
       </c>
@@ -1350,7 +1310,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" hidden="1">
       <c r="A33" s="1">
         <v>0</v>
       </c>
@@ -1373,7 +1333,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" hidden="1">
       <c r="A34" s="1">
         <v>0</v>
       </c>
@@ -1396,7 +1356,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" hidden="1">
       <c r="A35" s="1">
         <v>0</v>
       </c>
@@ -1416,7 +1376,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" hidden="1">
       <c r="A36" s="1">
         <v>0</v>
       </c>
@@ -1436,7 +1396,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" s="1">
         <v>0</v>
       </c>
@@ -1457,7 +1417,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G36"/>
+  <autoFilter ref="A1:G37">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Todos"/>
+        <filter val="Vagner"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:F33">
     <sortCondition descending="1" ref="A2"/>
   </sortState>

</xml_diff>

<commit_message>
Atualização WBS e tarefas
Atualização WBS e tarefas
</commit_message>
<xml_diff>
--- a/TCC/2º Encontro/Tarefas.xlsx
+++ b/TCC/2º Encontro/Tarefas.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="62">
   <si>
     <t>Tarefa</t>
   </si>
@@ -210,6 +210,21 @@
       </rPr>
       <t>Na última versão tinhamos o quadro de stakeholrders/ usuário, porém não vi nesse versão, removemos ele?</t>
     </r>
+  </si>
+  <si>
+    <t>Susbsistema serviço será excluído</t>
+  </si>
+  <si>
+    <t>Susbsistema empresa foi atualizado, consultar wbs para verificar atualizações</t>
+  </si>
+  <si>
+    <t>Análise realizada, subsistemas controle de acesso e empresa sofreram alterações, verificar no wbs</t>
+  </si>
+  <si>
+    <t>Padronização realizada</t>
+  </si>
+  <si>
+    <t>Nomenclatura padronizada no WBS</t>
   </si>
 </sst>
 </file>
@@ -276,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -292,6 +307,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,11 +613,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -611,11 +630,11 @@
     <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="28.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" style="4" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="22.5">
+    <row r="1" spans="1:8" s="5" customFormat="1" ht="22.5">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
@@ -637,8 +656,9 @@
       <c r="G1" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" hidden="1">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -660,8 +680,9 @@
       <c r="G2" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" hidden="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -683,8 +704,9 @@
       <c r="G3" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -706,8 +728,9 @@
       <c r="G4" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="22.5">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="33.75">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -727,10 +750,13 @@
         <v>42933</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="22.5">
+        <v>51</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="22.5">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -750,10 +776,13 @@
         <v>42933</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="33.75">
+        <v>51</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="33.75">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -775,8 +804,9 @@
       <c r="G7" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" hidden="1">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -798,8 +828,9 @@
       <c r="G8" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" hidden="1">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -818,8 +849,9 @@
       <c r="G9" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" hidden="1">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -841,8 +873,9 @@
       <c r="G10" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" hidden="1">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -864,8 +897,9 @@
       <c r="G11" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" hidden="1">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -887,8 +921,9 @@
       <c r="G12" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" hidden="1">
       <c r="A13" s="1">
         <v>0</v>
       </c>
@@ -910,8 +945,9 @@
       <c r="G13" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" hidden="1">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -933,8 +969,9 @@
       <c r="G14" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" hidden="1">
       <c r="A15" s="1">
         <v>0</v>
       </c>
@@ -956,8 +993,9 @@
       <c r="G15" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="1:8" hidden="1">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -979,8 +1017,9 @@
       <c r="G16" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="22.5">
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="1:8" ht="22.5">
       <c r="A17" s="1">
         <v>0</v>
       </c>
@@ -1002,8 +1041,9 @@
       <c r="G17" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="1:8" ht="33.75">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -1023,10 +1063,13 @@
         <v>42933</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="22.5">
+        <v>51</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="22.5">
       <c r="A19" s="1">
         <v>0</v>
       </c>
@@ -1046,10 +1089,13 @@
         <v>42933</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>51</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" hidden="1">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1071,8 +1117,9 @@
       <c r="G20" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20" s="8"/>
+    </row>
+    <row r="21" spans="1:8" hidden="1">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -1094,8 +1141,9 @@
       <c r="G21" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21" s="8"/>
+    </row>
+    <row r="22" spans="1:8" hidden="1">
       <c r="A22" s="1">
         <v>0</v>
       </c>
@@ -1117,8 +1165,9 @@
       <c r="G22" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22" s="8"/>
+    </row>
+    <row r="23" spans="1:8" hidden="1">
       <c r="A23" s="1">
         <v>0</v>
       </c>
@@ -1140,8 +1189,9 @@
       <c r="G23" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" s="8"/>
+    </row>
+    <row r="24" spans="1:8" hidden="1">
       <c r="A24" s="1">
         <v>0</v>
       </c>
@@ -1163,8 +1213,9 @@
       <c r="G24" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="22.5">
+      <c r="H24" s="8"/>
+    </row>
+    <row r="25" spans="1:8" ht="22.5">
       <c r="A25" s="1">
         <v>0</v>
       </c>
@@ -1186,8 +1237,9 @@
       <c r="G25" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="22.5">
+      <c r="H25" s="8"/>
+    </row>
+    <row r="26" spans="1:8" ht="22.5" hidden="1">
       <c r="A26" s="1">
         <v>0</v>
       </c>
@@ -1209,8 +1261,9 @@
       <c r="G26" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26" s="8"/>
+    </row>
+    <row r="27" spans="1:8" hidden="1">
       <c r="A27" s="1">
         <v>0</v>
       </c>
@@ -1232,8 +1285,9 @@
       <c r="G27" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27" s="8"/>
+    </row>
+    <row r="28" spans="1:8" hidden="1">
       <c r="A28" s="1">
         <v>0</v>
       </c>
@@ -1255,8 +1309,9 @@
       <c r="G28" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="1:8" hidden="1">
       <c r="A29" s="1">
         <v>0</v>
       </c>
@@ -1278,8 +1333,9 @@
       <c r="G29" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" spans="1:8" hidden="1">
       <c r="A30" s="1">
         <v>0</v>
       </c>
@@ -1301,8 +1357,9 @@
       <c r="G30" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30" s="8"/>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1">
         <v>0</v>
       </c>
@@ -1322,10 +1379,13 @@
         <v>42933</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>51</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" hidden="1">
       <c r="A32" s="1">
         <v>0</v>
       </c>
@@ -1347,8 +1407,9 @@
       <c r="G32" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" hidden="1">
       <c r="A33" s="1">
         <v>0</v>
       </c>
@@ -1370,8 +1431,9 @@
       <c r="G33" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" hidden="1">
       <c r="A34" s="1">
         <v>0</v>
       </c>
@@ -1393,8 +1455,9 @@
       <c r="G34" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" hidden="1">
       <c r="A35" s="1">
         <v>0</v>
       </c>
@@ -1413,8 +1476,9 @@
       <c r="G35" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="56.25">
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" ht="56.25" hidden="1">
       <c r="A36" s="1">
         <v>0</v>
       </c>
@@ -1437,7 +1501,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" hidden="1">
       <c r="A37" s="1">
         <v>0</v>
       </c>
@@ -1456,8 +1520,9 @@
       <c r="G37" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" hidden="1">
       <c r="A38" s="1">
         <v>0</v>
       </c>
@@ -1476,8 +1541,16 @@
       <c r="G38" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="H38" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H38">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Vagner"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:F33">
     <sortCondition descending="1" ref="A2"/>
   </sortState>

</xml_diff>